<commit_message>
framework OK - excel sheet structure and all the repoert and code is ok
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestSuite.xlsx
+++ b/src/main/resources/testdata/TestSuite.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\JavaProjects\apitesting\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F36785-60DF-4DC4-AE51-58EE8A2002E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C236588D-937B-46E8-8BA9-F21A94F3CF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="2" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="1" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
     <sheet name="Keywords" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>TestID</t>
   </si>
@@ -77,18 +77,9 @@
     <t>ExpectedStatus</t>
   </si>
   <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>Execute POST request</t>
-  </si>
-  <si>
     <t>VERIFY_STATUS</t>
   </si>
   <si>
-    <t>Execute GET request</t>
-  </si>
-  <si>
     <t>Get Posts</t>
   </si>
   <si>
@@ -218,43 +209,34 @@
     <t>Hello-World</t>
   </si>
   <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>Verify response status is 200</t>
-  </si>
-  <si>
-    <t>VERIFY_JSON_PATH</t>
-  </si>
-  <si>
-    <t>Verify post title</t>
-  </si>
-  <si>
-    <t>Verify response status is 201</t>
-  </si>
-  <si>
-    <t>Verify user name in response</t>
-  </si>
-  <si>
-    <t>Verify user email</t>
-  </si>
-  <si>
-    <t>Verify capital city</t>
-  </si>
-  <si>
-    <t>Verify city name</t>
-  </si>
-  <si>
-    <t>Verify repository name</t>
-  </si>
-  <si>
-    <t>/data/2.5/weather?q=London&amp;appid=6aa6cd8c45d248d374aac371cdf096b1</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>title</t>
+    <t>Keyword1</t>
+  </si>
+  <si>
+    <t>Keyword2</t>
+  </si>
+  <si>
+    <t>Keyword3</t>
+  </si>
+  <si>
+    <t>AuthRequired</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>/data/2.5/weather?q=London&amp;appid=6aa6cd8c45d248d374aac371cd</t>
+  </si>
+  <si>
+    <t>API_CALL</t>
+  </si>
+  <si>
+    <t>VERIFY_RESPONSE</t>
+  </si>
+  <si>
+    <t>$.title</t>
   </si>
 </sst>
 </file>
@@ -609,6 +591,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFFC6CA-DB32-4362-BDA5-12E02F8A4EBF}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -638,7 +817,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>12</v>
@@ -647,10 +826,10 @@
         <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -658,26 +837,28 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G2" s="2">
         <v>200</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -685,136 +866,144 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G3" s="2">
         <v>201</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G4" s="2">
         <v>200</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G5" s="2">
         <v>200</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G6" s="2">
         <v>200</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G7" s="2">
         <v>200</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -822,25 +1011,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{48D0534A-3B00-4C3D-B8CB-E660BCE73B73}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://reqres.in/" xr:uid="{39428DFF-0B46-43B0-9232-3F380D008083}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://reqres.in/" xr:uid="{A69AB898-5038-4EDE-9C74-91DFEEC96031}"/>
-    <hyperlink ref="I4" r:id="rId4" display="mailto:janet.weaver@reqres.in" xr:uid="{9410A8DF-63AC-4A1C-80BB-F15AC5B09F91}"/>
-    <hyperlink ref="B5" r:id="rId5" display="https://restcountries.com/" xr:uid="{C76111C6-BF7A-4D93-A65E-35900824EA80}"/>
-    <hyperlink ref="B6" r:id="rId6" display="https://api.openweathermap.org/" xr:uid="{C5B0F835-F75C-4AD6-874B-D4D797C93E27}"/>
-    <hyperlink ref="B7" r:id="rId7" display="https://api.github.com/" xr:uid="{6D759445-879D-4083-A164-BEED04FAB393}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://jsonplaceholder.typicode.com/" xr:uid="{5287201B-8F7E-491A-9063-3461685A46C0}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://reqres.in/" xr:uid="{EDD9AB1A-B6D3-4F74-B6CB-0AB313516DA5}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://reqres.in/" xr:uid="{81DC841D-2818-4857-8CB2-E90F2216EF63}"/>
+    <hyperlink ref="I4" r:id="rId4" display="mailto:janet.weaver@reqres.in" xr:uid="{86606544-7434-4E4D-ABED-7FB4B45CD2E6}"/>
+    <hyperlink ref="B5" r:id="rId5" display="https://restcountries.com/" xr:uid="{F948242F-DD3D-4001-9AF6-CA7F4A7BD298}"/>
+    <hyperlink ref="B6" r:id="rId6" display="https://api.openweathermap.org/" xr:uid="{D543C442-1878-48CD-AC56-B0F0F93BAF0F}"/>
+    <hyperlink ref="B7" r:id="rId7" display="https://api.github.com/" xr:uid="{6698C00C-4620-49FD-B015-DD7D1AE50D86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127D1E2E-376C-4614-81B4-808F21CEC111}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D7"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,400 +1039,177 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127D1E2E-376C-4614-81B4-808F21CEC111}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Request Body structure in the data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestSuite.xlsx
+++ b/src/main/resources/testdata/TestSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\JavaProjects\apitesting\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C236588D-937B-46E8-8BA9-F21A94F3CF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFE6449-65B8-4A3F-AF96-F090E30A877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>TestID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>RequestBody</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>/api/users</t>
   </si>
   <si>
-    <t>{"name": "John Doe","job": "QA Lead"}</t>
-  </si>
-  <si>
     <t>$.name</t>
   </si>
   <si>
@@ -237,6 +231,24 @@
   </si>
   <si>
     <t>$.title</t>
+  </si>
+  <si>
+    <t>RequestBodyKey</t>
+  </si>
+  <si>
+    <t>RequestBodyValue</t>
+  </si>
+  <si>
+    <t>name, job</t>
+  </si>
+  <si>
+    <t>John Doe, QA Lead</t>
+  </si>
+  <si>
+    <t>tcid.id, dob.lastdob</t>
+  </si>
+  <si>
+    <t>jj3, 77-09-9</t>
   </si>
 </sst>
 </file>
@@ -617,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -631,10 +643,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -643,7 +655,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -657,13 +669,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -680,19 +692,19 @@
     </row>
     <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
@@ -706,22 +718,22 @@
     </row>
     <row r="5" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -732,19 +744,19 @@
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>6</v>
@@ -758,19 +770,19 @@
     </row>
     <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
@@ -789,21 +801,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFFC6CA-DB32-4362-BDA5-12E02F8A4EBF}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="3" max="3" width="51.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,204 +829,229 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2">
+        <v>200</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="2">
-        <v>200</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2">
+        <v>201</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="2">
-        <v>201</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="2">
+        <v>200</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="2">
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="2">
         <v>200</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="2">
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="2">
         <v>200</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2">
         <v>200</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="2">
-        <v>200</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://jsonplaceholder.typicode.com/" xr:uid="{5287201B-8F7E-491A-9063-3461685A46C0}"/>
     <hyperlink ref="B3" r:id="rId2" display="https://reqres.in/" xr:uid="{EDD9AB1A-B6D3-4F74-B6CB-0AB313516DA5}"/>
     <hyperlink ref="B4" r:id="rId3" display="https://reqres.in/" xr:uid="{81DC841D-2818-4857-8CB2-E90F2216EF63}"/>
-    <hyperlink ref="I4" r:id="rId4" display="mailto:janet.weaver@reqres.in" xr:uid="{86606544-7434-4E4D-ABED-7FB4B45CD2E6}"/>
+    <hyperlink ref="J4" r:id="rId4" display="mailto:janet.weaver@reqres.in" xr:uid="{86606544-7434-4E4D-ABED-7FB4B45CD2E6}"/>
     <hyperlink ref="B5" r:id="rId5" display="https://restcountries.com/" xr:uid="{F948242F-DD3D-4001-9AF6-CA7F4A7BD298}"/>
     <hyperlink ref="B6" r:id="rId6" display="https://api.openweathermap.org/" xr:uid="{D543C442-1878-48CD-AC56-B0F0F93BAF0F}"/>
     <hyperlink ref="B7" r:id="rId7" display="https://api.github.com/" xr:uid="{6698C00C-4620-49FD-B015-DD7D1AE50D86}"/>
@@ -1039,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -1054,13 +1091,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1069,73 +1106,73 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2"/>
     </row>

</xml_diff>